<commit_message>
Create CommonOutputSteps and reuse through scenarios
</commit_message>
<xml_diff>
--- a/SpecFlowExample/SpecFlowExample.feature.xlsx
+++ b/SpecFlowExample/SpecFlowExample.feature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MultiplicationTests" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Use</t>
   </si>
@@ -29,12 +29,6 @@
     <t>I calculate multiplication</t>
   </si>
   <si>
-    <t>&lt;MultiplicationOut&gt;</t>
-  </si>
-  <si>
-    <t>Output Multiplication is</t>
-  </si>
-  <si>
     <t>case</t>
   </si>
   <si>
@@ -44,9 +38,6 @@
     <t>inputValue</t>
   </si>
   <si>
-    <t>MultiplicationOut</t>
-  </si>
-  <si>
     <t>Given</t>
   </si>
   <si>
@@ -68,13 +59,13 @@
     <t>I calculate addition</t>
   </si>
   <si>
-    <t>Output Addition is</t>
-  </si>
-  <si>
-    <t>&lt;AdditionOut&gt;</t>
-  </si>
-  <si>
-    <t>AdditionOut</t>
+    <t>&lt;ResultOut&gt;</t>
+  </si>
+  <si>
+    <t>ResultOut</t>
+  </si>
+  <si>
+    <t>Result is</t>
   </si>
 </sst>
 </file>
@@ -462,7 +453,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +465,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -488,7 +479,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -496,13 +487,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -513,25 +504,25 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -542,7 +533,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -553,7 +544,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -572,7 +563,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +575,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -598,21 +589,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -623,25 +614,25 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -652,7 +643,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -663,7 +654,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>0</v>

</xml_diff>